<commit_message>
updates to .toml, readme, data
</commit_message>
<xml_diff>
--- a/tests/day3.xlsx
+++ b/tests/day3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pnnl-my.sharepoint.com/personal/phil_parisi_pnnl_gov/Documents/Documents/PNNL/PhilRepo/ClimateSimulation/rpi/static/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pnnl-my.sharepoint.com/personal/phil_parisi_pnnl_gov/Documents/Documents/PNNL/PhilRepo/ClimateSimulation/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="38" documentId="8_{2138AAD7-D236-A646-8728-8798ABC91DCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2CA0F4FD-A0B9-104F-85C0-50FD3610F123}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="760" windowWidth="28040" windowHeight="16960" xr2:uid="{DE3C112F-27B3-434E-943A-F435A4ED6234}"/>
+    <workbookView minimized="1" xWindow="940" yWindow="760" windowWidth="28040" windowHeight="16960" xr2:uid="{DE3C112F-27B3-434E-943A-F435A4ED6234}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="h:mm:ss;@"/>
+    <numFmt numFmtId="164" formatCode="h:mm:ss;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -83,7 +83,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -99,6 +99,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -440,7 +444,7 @@
       </c>
       <c r="B2">
         <f ca="1">RANDBETWEEN(0,100)</f>
-        <v>2</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -449,7 +453,7 @@
       </c>
       <c r="B3">
         <f t="shared" ref="B3:B66" ca="1" si="0">RANDBETWEEN(0,100)</f>
-        <v>7</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -458,7 +462,7 @@
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>21</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -467,7 +471,7 @@
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -476,7 +480,7 @@
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>92</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -485,7 +489,7 @@
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -494,7 +498,7 @@
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>67</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -503,7 +507,7 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>33</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -512,7 +516,7 @@
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>98</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -521,7 +525,7 @@
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>78</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -530,7 +534,7 @@
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -539,7 +543,7 @@
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>58</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -548,7 +552,7 @@
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -557,7 +561,7 @@
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>25</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -566,7 +570,7 @@
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -575,7 +579,7 @@
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -584,7 +588,7 @@
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="0"/>
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -593,7 +597,7 @@
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="0"/>
-        <v>51</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -602,7 +606,7 @@
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="0"/>
-        <v>92</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -611,7 +615,7 @@
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -620,7 +624,7 @@
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="0"/>
-        <v>70</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -629,7 +633,7 @@
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="0"/>
-        <v>50</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -638,7 +642,7 @@
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -647,7 +651,7 @@
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="0"/>
-        <v>74</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -656,7 +660,7 @@
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -665,7 +669,7 @@
       </c>
       <c r="B27">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -674,7 +678,7 @@
       </c>
       <c r="B28">
         <f t="shared" ca="1" si="0"/>
-        <v>28</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -683,7 +687,7 @@
       </c>
       <c r="B29">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -692,7 +696,7 @@
       </c>
       <c r="B30">
         <f t="shared" ca="1" si="0"/>
-        <v>90</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -701,7 +705,7 @@
       </c>
       <c r="B31">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -710,7 +714,7 @@
       </c>
       <c r="B32">
         <f t="shared" ca="1" si="0"/>
-        <v>55</v>
+        <v>85</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -719,7 +723,7 @@
       </c>
       <c r="B33">
         <f t="shared" ca="1" si="0"/>
-        <v>58</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -728,7 +732,7 @@
       </c>
       <c r="B34">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -737,7 +741,7 @@
       </c>
       <c r="B35">
         <f t="shared" ca="1" si="0"/>
-        <v>46</v>
+        <v>9</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -746,7 +750,7 @@
       </c>
       <c r="B36">
         <f t="shared" ca="1" si="0"/>
-        <v>29</v>
+        <v>73</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
@@ -755,7 +759,7 @@
       </c>
       <c r="B37">
         <f t="shared" ca="1" si="0"/>
-        <v>95</v>
+        <v>87</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
@@ -764,7 +768,7 @@
       </c>
       <c r="B38">
         <f t="shared" ca="1" si="0"/>
-        <v>76</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
@@ -782,7 +786,7 @@
       </c>
       <c r="B40">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>79</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
@@ -791,7 +795,7 @@
       </c>
       <c r="B41">
         <f t="shared" ca="1" si="0"/>
-        <v>49</v>
+        <v>94</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
@@ -800,7 +804,7 @@
       </c>
       <c r="B42">
         <f t="shared" ca="1" si="0"/>
-        <v>89</v>
+        <v>13</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
@@ -809,7 +813,7 @@
       </c>
       <c r="B43">
         <f t="shared" ca="1" si="0"/>
-        <v>23</v>
+        <v>75</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
@@ -818,7 +822,7 @@
       </c>
       <c r="B44">
         <f t="shared" ca="1" si="0"/>
-        <v>59</v>
+        <v>33</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
@@ -827,7 +831,7 @@
       </c>
       <c r="B45">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
@@ -836,7 +840,7 @@
       </c>
       <c r="B46">
         <f t="shared" ca="1" si="0"/>
-        <v>79</v>
+        <v>33</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
@@ -845,7 +849,7 @@
       </c>
       <c r="B47">
         <f t="shared" ca="1" si="0"/>
-        <v>50</v>
+        <v>26</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
@@ -854,7 +858,7 @@
       </c>
       <c r="B48">
         <f t="shared" ca="1" si="0"/>
-        <v>30</v>
+        <v>95</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
@@ -863,7 +867,7 @@
       </c>
       <c r="B49">
         <f t="shared" ca="1" si="0"/>
-        <v>60</v>
+        <v>69</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
@@ -872,7 +876,7 @@
       </c>
       <c r="B50">
         <f t="shared" ca="1" si="0"/>
-        <v>85</v>
+        <v>64</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
@@ -881,7 +885,7 @@
       </c>
       <c r="B51">
         <f t="shared" ca="1" si="0"/>
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
@@ -890,7 +894,7 @@
       </c>
       <c r="B52">
         <f t="shared" ca="1" si="0"/>
-        <v>47</v>
+        <v>90</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
@@ -899,7 +903,7 @@
       </c>
       <c r="B53">
         <f t="shared" ca="1" si="0"/>
-        <v>22</v>
+        <v>61</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
@@ -908,7 +912,7 @@
       </c>
       <c r="B54">
         <f t="shared" ca="1" si="0"/>
-        <v>37</v>
+        <v>7</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
@@ -917,7 +921,7 @@
       </c>
       <c r="B55">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
@@ -926,7 +930,7 @@
       </c>
       <c r="B56">
         <f t="shared" ca="1" si="0"/>
-        <v>94</v>
+        <v>51</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
@@ -935,7 +939,7 @@
       </c>
       <c r="B57">
         <f t="shared" ca="1" si="0"/>
-        <v>89</v>
+        <v>33</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
@@ -944,7 +948,7 @@
       </c>
       <c r="B58">
         <f t="shared" ca="1" si="0"/>
-        <v>35</v>
+        <v>91</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
@@ -953,7 +957,7 @@
       </c>
       <c r="B59">
         <f t="shared" ca="1" si="0"/>
-        <v>61</v>
+        <v>11</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
@@ -962,7 +966,7 @@
       </c>
       <c r="B60">
         <f t="shared" ca="1" si="0"/>
-        <v>43</v>
+        <v>76</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
@@ -971,7 +975,7 @@
       </c>
       <c r="B61">
         <f t="shared" ca="1" si="0"/>
-        <v>25</v>
+        <v>90</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
@@ -980,7 +984,7 @@
       </c>
       <c r="B62">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
@@ -989,7 +993,7 @@
       </c>
       <c r="B63">
         <f t="shared" ca="1" si="0"/>
-        <v>35</v>
+        <v>15</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
@@ -998,7 +1002,7 @@
       </c>
       <c r="B64">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>68</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
@@ -1007,7 +1011,7 @@
       </c>
       <c r="B65">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>70</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
@@ -1016,7 +1020,7 @@
       </c>
       <c r="B66">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>42</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
@@ -1025,7 +1029,7 @@
       </c>
       <c r="B67">
         <f t="shared" ref="B67:B130" ca="1" si="1">RANDBETWEEN(0,100)</f>
-        <v>20</v>
+        <v>46</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
@@ -1034,7 +1038,7 @@
       </c>
       <c r="B68">
         <f t="shared" ca="1" si="1"/>
-        <v>38</v>
+        <v>91</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
@@ -1043,7 +1047,7 @@
       </c>
       <c r="B69">
         <f t="shared" ca="1" si="1"/>
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
@@ -1052,7 +1056,7 @@
       </c>
       <c r="B70">
         <f t="shared" ca="1" si="1"/>
-        <v>18</v>
+        <v>96</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
@@ -1061,7 +1065,7 @@
       </c>
       <c r="B71">
         <f t="shared" ca="1" si="1"/>
-        <v>29</v>
+        <v>63</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
@@ -1070,7 +1074,7 @@
       </c>
       <c r="B72">
         <f t="shared" ca="1" si="1"/>
-        <v>12</v>
+        <v>63</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
@@ -1079,7 +1083,7 @@
       </c>
       <c r="B73">
         <f t="shared" ca="1" si="1"/>
-        <v>95</v>
+        <v>43</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
@@ -1088,7 +1092,7 @@
       </c>
       <c r="B74">
         <f t="shared" ca="1" si="1"/>
-        <v>35</v>
+        <v>91</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
@@ -1097,7 +1101,7 @@
       </c>
       <c r="B75">
         <f t="shared" ca="1" si="1"/>
-        <v>51</v>
+        <v>15</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
@@ -1106,7 +1110,7 @@
       </c>
       <c r="B76">
         <f t="shared" ca="1" si="1"/>
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
@@ -1115,7 +1119,7 @@
       </c>
       <c r="B77">
         <f t="shared" ca="1" si="1"/>
-        <v>44</v>
+        <v>10</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
@@ -1124,7 +1128,7 @@
       </c>
       <c r="B78">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
@@ -1133,7 +1137,7 @@
       </c>
       <c r="B79">
         <f t="shared" ca="1" si="1"/>
-        <v>35</v>
+        <v>66</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
@@ -1142,7 +1146,7 @@
       </c>
       <c r="B80">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>95</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
@@ -1151,7 +1155,7 @@
       </c>
       <c r="B81">
         <f t="shared" ca="1" si="1"/>
-        <v>37</v>
+        <v>13</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
@@ -1160,7 +1164,7 @@
       </c>
       <c r="B82">
         <f t="shared" ca="1" si="1"/>
-        <v>40</v>
+        <v>97</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
@@ -1169,7 +1173,7 @@
       </c>
       <c r="B83">
         <f t="shared" ca="1" si="1"/>
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
@@ -1178,7 +1182,7 @@
       </c>
       <c r="B84">
         <f t="shared" ca="1" si="1"/>
-        <v>68</v>
+        <v>31</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
@@ -1187,7 +1191,7 @@
       </c>
       <c r="B85">
         <f t="shared" ca="1" si="1"/>
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
@@ -1196,7 +1200,7 @@
       </c>
       <c r="B86">
         <f t="shared" ca="1" si="1"/>
-        <v>56</v>
+        <v>17</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
@@ -1205,7 +1209,7 @@
       </c>
       <c r="B87">
         <f t="shared" ca="1" si="1"/>
-        <v>28</v>
+        <v>92</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
@@ -1214,7 +1218,7 @@
       </c>
       <c r="B88">
         <f t="shared" ca="1" si="1"/>
-        <v>35</v>
+        <v>19</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
@@ -1223,7 +1227,7 @@
       </c>
       <c r="B89">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>55</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
@@ -1232,7 +1236,7 @@
       </c>
       <c r="B90">
         <f t="shared" ca="1" si="1"/>
-        <v>42</v>
+        <v>83</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
@@ -1241,7 +1245,7 @@
       </c>
       <c r="B91">
         <f t="shared" ca="1" si="1"/>
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
@@ -1250,7 +1254,7 @@
       </c>
       <c r="B92">
         <f t="shared" ca="1" si="1"/>
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
@@ -1259,7 +1263,7 @@
       </c>
       <c r="B93">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>34</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
@@ -1268,7 +1272,7 @@
       </c>
       <c r="B94">
         <f t="shared" ca="1" si="1"/>
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
@@ -1277,7 +1281,7 @@
       </c>
       <c r="B95">
         <f t="shared" ca="1" si="1"/>
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
@@ -1286,7 +1290,7 @@
       </c>
       <c r="B96">
         <f t="shared" ca="1" si="1"/>
-        <v>75</v>
+        <v>43</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
@@ -1295,7 +1299,7 @@
       </c>
       <c r="B97">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>53</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
@@ -1304,7 +1308,7 @@
       </c>
       <c r="B98">
         <f t="shared" ca="1" si="1"/>
-        <v>68</v>
+        <v>39</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
@@ -1313,7 +1317,7 @@
       </c>
       <c r="B99">
         <f t="shared" ca="1" si="1"/>
-        <v>84</v>
+        <v>94</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
@@ -1322,7 +1326,7 @@
       </c>
       <c r="B100">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>75</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
@@ -1331,7 +1335,7 @@
       </c>
       <c r="B101">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>91</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
@@ -1340,7 +1344,7 @@
       </c>
       <c r="B102">
         <f t="shared" ca="1" si="1"/>
-        <v>37</v>
+        <v>13</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
@@ -1349,7 +1353,7 @@
       </c>
       <c r="B103">
         <f t="shared" ca="1" si="1"/>
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
@@ -1358,7 +1362,7 @@
       </c>
       <c r="B104">
         <f t="shared" ca="1" si="1"/>
-        <v>81</v>
+        <v>23</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
@@ -1367,7 +1371,7 @@
       </c>
       <c r="B105">
         <f t="shared" ca="1" si="1"/>
-        <v>59</v>
+        <v>11</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
@@ -1376,7 +1380,7 @@
       </c>
       <c r="B106">
         <f t="shared" ca="1" si="1"/>
-        <v>63</v>
+        <v>71</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
@@ -1385,7 +1389,7 @@
       </c>
       <c r="B107">
         <f t="shared" ca="1" si="1"/>
-        <v>14</v>
+        <v>46</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
@@ -1394,7 +1398,7 @@
       </c>
       <c r="B108">
         <f t="shared" ca="1" si="1"/>
-        <v>85</v>
+        <v>71</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
@@ -1403,7 +1407,7 @@
       </c>
       <c r="B109">
         <f t="shared" ca="1" si="1"/>
-        <v>43</v>
+        <v>51</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
@@ -1412,7 +1416,7 @@
       </c>
       <c r="B110">
         <f t="shared" ca="1" si="1"/>
-        <v>65</v>
+        <v>80</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
@@ -1421,7 +1425,7 @@
       </c>
       <c r="B111">
         <f t="shared" ca="1" si="1"/>
-        <v>34</v>
+        <v>3</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
@@ -1430,7 +1434,7 @@
       </c>
       <c r="B112">
         <f t="shared" ca="1" si="1"/>
-        <v>27</v>
+        <v>8</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
@@ -1439,7 +1443,7 @@
       </c>
       <c r="B113">
         <f t="shared" ca="1" si="1"/>
-        <v>69</v>
+        <v>40</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
@@ -1448,7 +1452,7 @@
       </c>
       <c r="B114">
         <f t="shared" ca="1" si="1"/>
-        <v>13</v>
+        <v>83</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
@@ -1457,7 +1461,7 @@
       </c>
       <c r="B115">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>84</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
@@ -1466,7 +1470,7 @@
       </c>
       <c r="B116">
         <f t="shared" ca="1" si="1"/>
-        <v>93</v>
+        <v>35</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
@@ -1475,7 +1479,7 @@
       </c>
       <c r="B117">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>38</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
@@ -1484,7 +1488,7 @@
       </c>
       <c r="B118">
         <f t="shared" ca="1" si="1"/>
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
@@ -1493,7 +1497,7 @@
       </c>
       <c r="B119">
         <f t="shared" ca="1" si="1"/>
-        <v>89</v>
+        <v>12</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
@@ -1502,7 +1506,7 @@
       </c>
       <c r="B120">
         <f t="shared" ca="1" si="1"/>
-        <v>38</v>
+        <v>5</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
@@ -1511,7 +1515,7 @@
       </c>
       <c r="B121">
         <f t="shared" ca="1" si="1"/>
-        <v>42</v>
+        <v>67</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
@@ -1520,7 +1524,7 @@
       </c>
       <c r="B122">
         <f t="shared" ca="1" si="1"/>
-        <v>19</v>
+        <v>72</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
@@ -1529,7 +1533,7 @@
       </c>
       <c r="B123">
         <f t="shared" ca="1" si="1"/>
-        <v>45</v>
+        <v>10</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
@@ -1538,7 +1542,7 @@
       </c>
       <c r="B124">
         <f t="shared" ca="1" si="1"/>
-        <v>96</v>
+        <v>40</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
@@ -1547,7 +1551,7 @@
       </c>
       <c r="B125">
         <f t="shared" ca="1" si="1"/>
-        <v>45</v>
+        <v>76</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
@@ -1556,7 +1560,7 @@
       </c>
       <c r="B126">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>21</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
@@ -1565,7 +1569,7 @@
       </c>
       <c r="B127">
         <f t="shared" ca="1" si="1"/>
-        <v>38</v>
+        <v>52</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
@@ -1574,7 +1578,7 @@
       </c>
       <c r="B128">
         <f t="shared" ca="1" si="1"/>
-        <v>70</v>
+        <v>96</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
@@ -1583,7 +1587,7 @@
       </c>
       <c r="B129">
         <f t="shared" ca="1" si="1"/>
-        <v>39</v>
+        <v>11</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
@@ -1592,7 +1596,7 @@
       </c>
       <c r="B130">
         <f t="shared" ca="1" si="1"/>
-        <v>70</v>
+        <v>9</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
@@ -1601,7 +1605,7 @@
       </c>
       <c r="B131">
         <f t="shared" ref="B131:B145" ca="1" si="2">RANDBETWEEN(0,100)</f>
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
@@ -1610,7 +1614,7 @@
       </c>
       <c r="B132">
         <f t="shared" ca="1" si="2"/>
-        <v>59</v>
+        <v>4</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
@@ -1619,7 +1623,7 @@
       </c>
       <c r="B133">
         <f t="shared" ca="1" si="2"/>
-        <v>75</v>
+        <v>54</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
@@ -1628,7 +1632,7 @@
       </c>
       <c r="B134">
         <f t="shared" ca="1" si="2"/>
-        <v>39</v>
+        <v>23</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
@@ -1637,7 +1641,7 @@
       </c>
       <c r="B135">
         <f t="shared" ca="1" si="2"/>
-        <v>41</v>
+        <v>27</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
@@ -1646,7 +1650,7 @@
       </c>
       <c r="B136">
         <f t="shared" ca="1" si="2"/>
-        <v>85</v>
+        <v>22</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
@@ -1655,7 +1659,7 @@
       </c>
       <c r="B137">
         <f t="shared" ca="1" si="2"/>
-        <v>84</v>
+        <v>56</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
@@ -1664,7 +1668,7 @@
       </c>
       <c r="B138">
         <f t="shared" ca="1" si="2"/>
-        <v>43</v>
+        <v>32</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
@@ -1673,7 +1677,7 @@
       </c>
       <c r="B139">
         <f t="shared" ca="1" si="2"/>
-        <v>49</v>
+        <v>33</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
@@ -1682,7 +1686,7 @@
       </c>
       <c r="B140">
         <f t="shared" ca="1" si="2"/>
-        <v>18</v>
+        <v>96</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
@@ -1691,7 +1695,7 @@
       </c>
       <c r="B141">
         <f t="shared" ca="1" si="2"/>
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
@@ -1700,7 +1704,7 @@
       </c>
       <c r="B142">
         <f t="shared" ca="1" si="2"/>
-        <v>39</v>
+        <v>0</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
@@ -1709,7 +1713,7 @@
       </c>
       <c r="B143">
         <f t="shared" ca="1" si="2"/>
-        <v>92</v>
+        <v>59</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
@@ -1718,7 +1722,7 @@
       </c>
       <c r="B144">
         <f t="shared" ca="1" si="2"/>
-        <v>50</v>
+        <v>2</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
@@ -1727,7 +1731,7 @@
       </c>
       <c r="B145">
         <f t="shared" ca="1" si="2"/>
-        <v>52</v>
+        <v>43</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>